<commit_message>
Cambios realizados 26 octubre 2021
</commit_message>
<xml_diff>
--- a/WinTestService/DatosDeCarga/ArchivoCargarDatosCltes.xlsx
+++ b/WinTestService/DatosDeCarga/ArchivoCargarDatosCltes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garfi\source\repos\TestProcessExcelWithWcf\WinTestService\DatosDeCarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90CEA91-6F8A-4BA4-8BD9-71FC432C79BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F66C08-6E4A-41B5-A4E6-9DF1E4F7AB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C830E6CD-CDEC-4EAF-BAC5-F19EFA1A8278}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>codigo</t>
   </si>
@@ -48,7 +48,13 @@
     <t>Entidad</t>
   </si>
   <si>
-    <t>ClienteTest</t>
+    <t>CL_ClienteTest</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>AUTO</t>
   </si>
 </sst>
 </file>
@@ -400,27 +406,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EAE861-BD7C-451C-B771-A0D431FCA616}">
-  <dimension ref="B2:F36"/>
+  <dimension ref="B2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="102.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -431,7 +443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -445,10 +457,14 @@
       </c>
       <c r="F4" t="str">
         <f>"insert into " &amp;$C$2 &amp; " values (" &amp; C4&amp; ", '" &amp;D4 &amp; "','" &amp;E4 &amp; "');"</f>
-        <v>insert into ClienteTest values (1, 'Nombre1','Direccion1');</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (1, 'Nombre1','Direccion1');</v>
+      </c>
+      <c r="G4" t="str">
+        <f xml:space="preserve"> "wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, '" &amp;D4 &amp; "','" &amp;E4 &amp; "', 2, NULL, '" &amp;  $F$2 &amp;"', NULL);"</f>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre1','Direccion1', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -462,10 +478,14 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" ref="F5:F36" si="2">"insert into " &amp;$C$2 &amp; " values (" &amp; C5&amp; ", '" &amp;D5 &amp; "','" &amp;E5 &amp; "');"</f>
-        <v>insert into ClienteTest values (2, 'Nombre2','Direccion2');</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (2, 'Nombre2','Direccion2');</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G36" si="3" xml:space="preserve"> "wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, '" &amp;D5 &amp; "','" &amp;E5 &amp; "', 2, NULL, '" &amp;  $F$2 &amp;"', NULL);"</f>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre2','Direccion2', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -479,10 +499,14 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (3, 'Nombre3','Direccion3');</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (3, 'Nombre3','Direccion3');</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre3','Direccion3', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
@@ -496,10 +520,14 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (4, 'Nombre4','Direccion4');</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (4, 'Nombre4','Direccion4');</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre4','Direccion4', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -513,10 +541,14 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (5, 'Nombre5','Direccion5');</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (5, 'Nombre5','Direccion5');</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre5','Direccion5', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>6</v>
       </c>
@@ -530,10 +562,14 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (6, 'Nombre6','Direccion6');</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (6, 'Nombre6','Direccion6');</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre6','Direccion6', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>7</v>
       </c>
@@ -547,10 +583,14 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (7, 'Nombre7','Direccion7');</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (7, 'Nombre7','Direccion7');</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre7','Direccion7', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>8</v>
       </c>
@@ -564,10 +604,14 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (8, 'Nombre8','Direccion8');</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (8, 'Nombre8','Direccion8');</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre8','Direccion8', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>9</v>
       </c>
@@ -581,10 +625,14 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (9, 'Nombre9','Direccion9');</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (9, 'Nombre9','Direccion9');</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre9','Direccion9', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>10</v>
       </c>
@@ -598,10 +646,14 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (10, 'Nombre10','Direccion10');</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (10, 'Nombre10','Direccion10');</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre10','Direccion10', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>11</v>
       </c>
@@ -615,10 +667,14 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (11, 'Nombre11','Direccion11');</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (11, 'Nombre11','Direccion11');</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre11','Direccion11', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>12</v>
       </c>
@@ -632,10 +688,14 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (12, 'Nombre12','Direccion12');</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (12, 'Nombre12','Direccion12');</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre12','Direccion12', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>13</v>
       </c>
@@ -649,10 +709,14 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (13, 'Nombre13','Direccion13');</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (13, 'Nombre13','Direccion13');</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre13','Direccion13', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>14</v>
       </c>
@@ -666,10 +730,14 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (14, 'Nombre14','Direccion14');</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (14, 'Nombre14','Direccion14');</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre14','Direccion14', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>15</v>
       </c>
@@ -683,10 +751,14 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (15, 'Nombre15','Direccion15');</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (15, 'Nombre15','Direccion15');</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre15','Direccion15', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>16</v>
       </c>
@@ -700,10 +772,14 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (16, 'Nombre16','Direccion16');</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (16, 'Nombre16','Direccion16');</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre16','Direccion16', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>17</v>
       </c>
@@ -717,10 +793,14 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (17, 'Nombre17','Direccion17');</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (17, 'Nombre17','Direccion17');</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre17','Direccion17', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>18</v>
       </c>
@@ -734,10 +814,14 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (18, 'Nombre18','Direccion18');</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (18, 'Nombre18','Direccion18');</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre18','Direccion18', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>19</v>
       </c>
@@ -751,10 +835,14 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (19, 'Nombre19','Direccion19');</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (19, 'Nombre19','Direccion19');</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre19','Direccion19', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>20</v>
       </c>
@@ -768,10 +856,14 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (20, 'Nombre20','Direccion20');</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (20, 'Nombre20','Direccion20');</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre20','Direccion20', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>21</v>
       </c>
@@ -785,10 +877,14 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (21, 'Nombre21','Direccion21');</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (21, 'Nombre21','Direccion21');</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre21','Direccion21', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>22</v>
       </c>
@@ -802,10 +898,14 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (22, 'Nombre22','Direccion22');</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (22, 'Nombre22','Direccion22');</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre22','Direccion22', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>23</v>
       </c>
@@ -819,10 +919,14 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (23, 'Nombre23','Direccion23');</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (23, 'Nombre23','Direccion23');</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre23','Direccion23', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>24</v>
       </c>
@@ -836,10 +940,14 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (24, 'Nombre24','Direccion24');</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (24, 'Nombre24','Direccion24');</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre24','Direccion24', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>25</v>
       </c>
@@ -853,10 +961,14 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (25, 'Nombre25','Direccion25');</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (25, 'Nombre25','Direccion25');</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre25','Direccion25', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>26</v>
       </c>
@@ -870,10 +982,14 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (26, 'Nombre26','Direccion26');</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (26, 'Nombre26','Direccion26');</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre26','Direccion26', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>27</v>
       </c>
@@ -882,15 +998,19 @@
         <v>Nombre27</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" ref="E30:E36" si="3" xml:space="preserve"> "Direccion" &amp;C30</f>
+        <f t="shared" ref="E30:E36" si="4" xml:space="preserve"> "Direccion" &amp;C30</f>
         <v>Direccion27</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (27, 'Nombre27','Direccion27');</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (27, 'Nombre27','Direccion27');</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre27','Direccion27', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>28</v>
       </c>
@@ -899,15 +1019,19 @@
         <v>Nombre28</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Direccion28</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (28, 'Nombre28','Direccion28');</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (28, 'Nombre28','Direccion28');</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre28','Direccion28', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>29</v>
       </c>
@@ -916,15 +1040,19 @@
         <v>Nombre29</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Direccion29</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (29, 'Nombre29','Direccion29');</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (29, 'Nombre29','Direccion29');</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre29','Direccion29', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>30</v>
       </c>
@@ -933,15 +1061,19 @@
         <v>Nombre30</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Direccion30</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (30, 'Nombre30','Direccion30');</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (30, 'Nombre30','Direccion30');</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre30','Direccion30', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>31</v>
       </c>
@@ -950,15 +1082,19 @@
         <v>Nombre31</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Direccion31</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (31, 'Nombre31','Direccion31');</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (31, 'Nombre31','Direccion31');</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre31','Direccion31', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>32</v>
       </c>
@@ -967,15 +1103,19 @@
         <v>Nombre32</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Direccion32</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (32, 'Nombre32','Direccion32');</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+        <v>insert into CL_ClienteTest values (32, 'Nombre32','Direccion32');</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre32','Direccion32', 2, NULL, 'AUTO', NULL);</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>33</v>
       </c>
@@ -984,12 +1124,16 @@
         <v>Nombre33</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Direccion33</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="2"/>
-        <v>insert into ClienteTest values (33, 'Nombre33','Direccion33');</v>
+        <v>insert into CL_ClienteTest values (33, 'Nombre33','Direccion33');</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="3"/>
+        <v>wcod_cliente_n := null; CL_PCLIENTETEST.INSERTA (wcod_cliente_n, 'Nombre33','Direccion33', 2, NULL, 'AUTO', NULL);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>